<commit_message>
update solution for Q.three'
</commit_message>
<xml_diff>
--- a/附件四：354个操作变量信息.xlsx
+++ b/附件四：354个操作变量信息.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryuchen/Desktop/2020年B题/数模题/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D131165-4EB1-AD48-BE75-6C445F58223E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="3020" windowWidth="19440" windowHeight="15000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4772" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="986">
   <si>
     <t>S-ZORB.CAL_H2.PV</t>
   </si>
@@ -3532,8 +3533,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3668,7 +3669,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 4" xfId="1"/>
+    <cellStyle name="常规 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3945,27 +3946,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B326" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B332" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F338" sqref="F338"/>
+      <selection pane="bottomRight" activeCell="H341" sqref="H341"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="31.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="2"/>
+    <col min="6" max="6" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>979</v>
       </c>
@@ -3985,7 +3986,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4002,7 +4003,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4022,7 +4023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4042,7 +4043,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4062,7 +4063,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4082,7 +4083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4102,7 +4103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4122,7 +4123,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4142,7 +4143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="14" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4162,7 +4163,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4182,7 +4183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4202,7 +4203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4222,7 +4223,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4242,7 +4243,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4262,7 +4263,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4282,7 +4283,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4302,7 +4303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4322,7 +4323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4342,7 +4343,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4362,7 +4363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4382,7 +4383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4402,7 +4403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4422,7 +4423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4442,7 +4443,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4462,7 +4463,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4482,7 +4483,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4502,7 +4503,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4522,7 +4523,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4542,7 +4543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -4562,7 +4563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -4582,7 +4583,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4602,7 +4603,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -4622,7 +4623,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -4642,7 +4643,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -4662,7 +4663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -4682,7 +4683,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -4702,7 +4703,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4722,7 +4723,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -4742,7 +4743,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4762,7 +4763,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -4782,7 +4783,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -4802,7 +4803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -4822,7 +4823,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -4842,7 +4843,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -4862,7 +4863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -4882,7 +4883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -4902,7 +4903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -4922,7 +4923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -4942,7 +4943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -4962,7 +4963,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -4982,7 +4983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -5002,7 +5003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -5022,7 +5023,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -5042,7 +5043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -5062,7 +5063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -5082,7 +5083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -5102,7 +5103,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -5122,7 +5123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -5142,7 +5143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -5159,7 +5160,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -5179,7 +5180,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -5199,7 +5200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -5219,7 +5220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -5236,7 +5237,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -5256,7 +5257,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -5276,7 +5277,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -5296,7 +5297,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -5316,7 +5317,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -5336,7 +5337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -5356,7 +5357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -5376,7 +5377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -5396,7 +5397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -5416,7 +5417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -5436,7 +5437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -5456,7 +5457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -5476,7 +5477,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -5496,7 +5497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -5516,7 +5517,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -5536,7 +5537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -5556,7 +5557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -5576,7 +5577,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -5596,7 +5597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -5616,7 +5617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -5636,7 +5637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -5656,7 +5657,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -5676,7 +5677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5696,7 +5697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5713,7 +5714,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5727,7 +5728,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -5741,7 +5742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5755,7 +5756,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -5769,7 +5770,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5783,7 +5784,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -5797,7 +5798,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5811,7 +5812,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -5825,7 +5826,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="15">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -5845,7 +5846,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -5859,7 +5860,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -5873,7 +5874,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -5887,7 +5888,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -5901,7 +5902,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -5915,7 +5916,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -5929,7 +5930,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -5943,7 +5944,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -5957,7 +5958,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -5971,7 +5972,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -5982,7 +5983,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="15">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -6002,7 +6003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -6022,7 +6023,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -6036,7 +6037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -6050,7 +6051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -6064,7 +6065,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -6078,7 +6079,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="15">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -6098,7 +6099,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -6115,7 +6116,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -6135,7 +6136,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -6155,7 +6156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -6175,7 +6176,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -6195,7 +6196,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -6215,7 +6216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -6235,7 +6236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -6255,7 +6256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -6275,7 +6276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -6295,7 +6296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -6315,7 +6316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -6335,7 +6336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="15">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -6355,7 +6356,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -6372,7 +6373,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -6389,7 +6390,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -6409,7 +6410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -6426,7 +6427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -6446,7 +6447,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -6466,7 +6467,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -6486,7 +6487,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -6506,7 +6507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="15">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -6526,7 +6527,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -6546,7 +6547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -6566,7 +6567,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -6583,7 +6584,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -6600,7 +6601,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -6620,7 +6621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -6640,7 +6641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -6660,7 +6661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -6677,7 +6678,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -6694,7 +6695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -6711,7 +6712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -6731,7 +6732,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -6748,7 +6749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -6765,7 +6766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -6782,7 +6783,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -6799,7 +6800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -6816,7 +6817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -6836,7 +6837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -6853,7 +6854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -6870,7 +6871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -6890,7 +6891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -6907,7 +6908,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -6924,7 +6925,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -6941,7 +6942,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -6958,7 +6959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -6975,7 +6976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -6995,7 +6996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -7012,7 +7013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="15">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -7032,7 +7033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="15">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -7052,7 +7053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -7072,7 +7073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -7092,7 +7093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -7109,7 +7110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -7129,7 +7130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -7149,7 +7150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -7166,7 +7167,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -7186,7 +7187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -7206,7 +7207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -7226,7 +7227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -7246,7 +7247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -7260,7 +7261,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -7277,7 +7278,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -7294,7 +7295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -7311,7 +7312,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -7331,7 +7332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -7351,7 +7352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -7371,7 +7372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -7388,7 +7389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -7405,7 +7406,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -7422,7 +7423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -7439,7 +7440,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -7456,7 +7457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -7476,7 +7477,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -7493,7 +7494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -7510,7 +7511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -7530,7 +7531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -7550,7 +7551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -7570,7 +7571,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -7587,7 +7588,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -7607,7 +7608,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -7624,7 +7625,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -7644,7 +7645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" ht="15">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -7664,7 +7665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -7681,7 +7682,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -7698,7 +7699,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -7718,7 +7719,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -7738,7 +7739,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -7758,7 +7759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -7778,7 +7779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -7795,7 +7796,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -7812,7 +7813,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -7829,7 +7830,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" ht="15">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -7849,7 +7850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="15">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -7869,7 +7870,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -7886,7 +7887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -7903,7 +7904,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -7920,7 +7921,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -7940,7 +7941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -7957,7 +7958,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -7974,7 +7975,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -7991,7 +7992,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -8008,7 +8009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -8025,7 +8026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -8042,7 +8043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -8059,7 +8060,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -8076,7 +8077,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -8093,7 +8094,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -8110,7 +8111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -8127,7 +8128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -8144,7 +8145,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -8161,7 +8162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -8178,7 +8179,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -8195,7 +8196,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -8212,7 +8213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -8229,7 +8230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -8249,7 +8250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -8269,7 +8270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -8289,7 +8290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -8306,7 +8307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -8323,7 +8324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -8343,7 +8344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -8360,7 +8361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -8380,7 +8381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -8400,7 +8401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -8420,7 +8421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -8440,7 +8441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -8457,7 +8458,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -8474,7 +8475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -8491,7 +8492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -8508,7 +8509,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -8528,7 +8529,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -8545,7 +8546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -8562,7 +8563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -8579,7 +8580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -8596,7 +8597,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -8613,7 +8614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6">
       <c r="A252" s="1">
         <v>251</v>
       </c>
@@ -8630,7 +8631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6">
       <c r="A253" s="1">
         <v>252</v>
       </c>
@@ -8647,7 +8648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6">
       <c r="A254" s="1">
         <v>253</v>
       </c>
@@ -8664,7 +8665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6">
       <c r="A255" s="1">
         <v>254</v>
       </c>
@@ -8681,7 +8682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6">
       <c r="A256" s="1">
         <v>255</v>
       </c>
@@ -8698,7 +8699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6">
       <c r="A257" s="1">
         <v>256</v>
       </c>
@@ -8715,7 +8716,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6">
       <c r="A258" s="1">
         <v>257</v>
       </c>
@@ -8732,7 +8733,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6">
       <c r="A259" s="1">
         <v>258</v>
       </c>
@@ -8749,7 +8750,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6">
       <c r="A260" s="1">
         <v>259</v>
       </c>
@@ -8769,7 +8770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6">
       <c r="A261" s="1">
         <v>260</v>
       </c>
@@ -8786,7 +8787,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6">
       <c r="A262" s="1">
         <v>261</v>
       </c>
@@ -8806,7 +8807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6">
       <c r="A263" s="1">
         <v>262</v>
       </c>
@@ -8823,7 +8824,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6">
       <c r="A264" s="1">
         <v>263</v>
       </c>
@@ -8843,7 +8844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6">
       <c r="A265" s="1">
         <v>264</v>
       </c>
@@ -8860,7 +8861,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6">
       <c r="A266" s="1">
         <v>265</v>
       </c>
@@ -8880,7 +8881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6">
       <c r="A267" s="1">
         <v>266</v>
       </c>
@@ -8897,7 +8898,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6">
       <c r="A268" s="1">
         <v>267</v>
       </c>
@@ -8917,7 +8918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6">
       <c r="A269" s="1">
         <v>268</v>
       </c>
@@ -8934,7 +8935,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6">
       <c r="A270" s="1">
         <v>269</v>
       </c>
@@ -8954,7 +8955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6">
       <c r="A271" s="1">
         <v>270</v>
       </c>
@@ -8971,7 +8972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6">
       <c r="A272" s="1">
         <v>271</v>
       </c>
@@ -8991,7 +8992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6">
       <c r="A273" s="1">
         <v>272</v>
       </c>
@@ -9008,7 +9009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6">
       <c r="A274" s="1">
         <v>273</v>
       </c>
@@ -9028,7 +9029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6">
       <c r="A275" s="1">
         <v>274</v>
       </c>
@@ -9048,7 +9049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6">
       <c r="A276" s="1">
         <v>275</v>
       </c>
@@ -9068,7 +9069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6">
       <c r="A277" s="1">
         <v>276</v>
       </c>
@@ -9085,7 +9086,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6">
       <c r="A278" s="1">
         <v>277</v>
       </c>
@@ -9102,7 +9103,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6">
       <c r="A279" s="1">
         <v>278</v>
       </c>
@@ -9122,7 +9123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6">
       <c r="A280" s="1">
         <v>279</v>
       </c>
@@ -9142,7 +9143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6">
       <c r="A281" s="1">
         <v>280</v>
       </c>
@@ -9162,7 +9163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6">
       <c r="A282" s="1">
         <v>281</v>
       </c>
@@ -9179,7 +9180,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6">
       <c r="A283" s="1">
         <v>282</v>
       </c>
@@ -9196,7 +9197,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6">
       <c r="A284" s="1">
         <v>283</v>
       </c>
@@ -9216,7 +9217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6">
       <c r="A285" s="1">
         <v>284</v>
       </c>
@@ -9233,7 +9234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6">
       <c r="A286" s="1">
         <v>285</v>
       </c>
@@ -9250,7 +9251,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6">
       <c r="A287" s="1">
         <v>286</v>
       </c>
@@ -9267,7 +9268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6">
       <c r="A288" s="1">
         <v>287</v>
       </c>
@@ -9287,7 +9288,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6">
       <c r="A289" s="1">
         <v>288</v>
       </c>
@@ -9304,7 +9305,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6">
       <c r="A290" s="1">
         <v>289</v>
       </c>
@@ -9321,7 +9322,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6">
       <c r="A291" s="1">
         <v>290</v>
       </c>
@@ -9338,7 +9339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6">
       <c r="A292" s="1">
         <v>291</v>
       </c>
@@ -9358,7 +9359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6">
       <c r="A293" s="1">
         <v>292</v>
       </c>
@@ -9378,7 +9379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6">
       <c r="A294" s="1">
         <v>293</v>
       </c>
@@ -9398,7 +9399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6">
       <c r="A295" s="1">
         <v>294</v>
       </c>
@@ -9418,7 +9419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" ht="15">
       <c r="A296" s="1">
         <v>295</v>
       </c>
@@ -9438,7 +9439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6">
       <c r="A297" s="1">
         <v>296</v>
       </c>
@@ -9458,7 +9459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6">
       <c r="A298" s="1">
         <v>297</v>
       </c>
@@ -9478,7 +9479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6">
       <c r="A299" s="1">
         <v>298</v>
       </c>
@@ -9495,7 +9496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6">
       <c r="A300" s="1">
         <v>299</v>
       </c>
@@ -9515,7 +9516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6">
       <c r="A301" s="1">
         <v>300</v>
       </c>
@@ -9535,7 +9536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6">
       <c r="A302" s="1">
         <v>301</v>
       </c>
@@ -9555,7 +9556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6">
       <c r="A303" s="1">
         <v>302</v>
       </c>
@@ -9572,7 +9573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6">
       <c r="A304" s="1">
         <v>303</v>
       </c>
@@ -9592,7 +9593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6">
       <c r="A305" s="1">
         <v>304</v>
       </c>
@@ -9612,7 +9613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6">
       <c r="A306" s="1">
         <v>305</v>
       </c>
@@ -9632,7 +9633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6">
       <c r="A307" s="1">
         <v>306</v>
       </c>
@@ -9652,7 +9653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6">
       <c r="A308" s="1">
         <v>307</v>
       </c>
@@ -9672,7 +9673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6">
       <c r="A309" s="1">
         <v>308</v>
       </c>
@@ -9692,7 +9693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6">
       <c r="A310" s="1">
         <v>309</v>
       </c>
@@ -9712,7 +9713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6">
       <c r="A311" s="1">
         <v>310</v>
       </c>
@@ -9732,7 +9733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6">
       <c r="A312" s="1">
         <v>311</v>
       </c>
@@ -9752,7 +9753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6">
       <c r="A313" s="1">
         <v>312</v>
       </c>
@@ -9772,7 +9773,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6">
       <c r="A314" s="1">
         <v>313</v>
       </c>
@@ -9789,7 +9790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6">
       <c r="A315" s="1">
         <v>314</v>
       </c>
@@ -9806,7 +9807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6">
       <c r="A316" s="1">
         <v>315</v>
       </c>
@@ -9823,7 +9824,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6">
       <c r="A317" s="1">
         <v>316</v>
       </c>
@@ -9840,7 +9841,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6">
       <c r="A318" s="1">
         <v>317</v>
       </c>
@@ -9857,7 +9858,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6">
       <c r="A319" s="1">
         <v>318</v>
       </c>
@@ -9874,7 +9875,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6">
       <c r="A320" s="1">
         <v>319</v>
       </c>
@@ -9891,7 +9892,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6">
       <c r="A321" s="1">
         <v>320</v>
       </c>
@@ -9908,7 +9909,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6">
       <c r="A322" s="1">
         <v>321</v>
       </c>
@@ -9925,7 +9926,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6">
       <c r="A323" s="1">
         <v>322</v>
       </c>
@@ -9942,7 +9943,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6">
       <c r="A324" s="1">
         <v>323</v>
       </c>
@@ -9959,7 +9960,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6">
       <c r="A325" s="1">
         <v>324</v>
       </c>
@@ -9976,7 +9977,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6">
       <c r="A326" s="1">
         <v>325</v>
       </c>
@@ -9993,7 +9994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6">
       <c r="A327" s="1">
         <v>326</v>
       </c>
@@ -10013,7 +10014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6">
       <c r="A328" s="1">
         <v>327</v>
       </c>
@@ -10033,7 +10034,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6">
       <c r="A329" s="1">
         <v>328</v>
       </c>
@@ -10050,7 +10051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6">
       <c r="A330" s="1">
         <v>329</v>
       </c>
@@ -10070,7 +10071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6">
       <c r="A331" s="1">
         <v>330</v>
       </c>
@@ -10090,7 +10091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6">
       <c r="A332" s="1">
         <v>331</v>
       </c>
@@ -10110,7 +10111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6">
       <c r="A333" s="1">
         <v>332</v>
       </c>
@@ -10127,7 +10128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6">
       <c r="A334" s="1">
         <v>333</v>
       </c>
@@ -10147,7 +10148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6">
       <c r="A335" s="1">
         <v>334</v>
       </c>
@@ -10167,7 +10168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6">
       <c r="A336" s="1">
         <v>335</v>
       </c>
@@ -10187,7 +10188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6">
       <c r="A337" s="1">
         <v>336</v>
       </c>
@@ -10207,7 +10208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6">
       <c r="A338" s="1">
         <v>337</v>
       </c>
@@ -10227,7 +10228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6">
       <c r="A339" s="1">
         <v>338</v>
       </c>
@@ -10247,7 +10248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6">
       <c r="A340" s="1">
         <v>339</v>
       </c>
@@ -10267,7 +10268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6">
       <c r="A341" s="1">
         <v>340</v>
       </c>
@@ -10287,7 +10288,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6">
       <c r="A342" s="1">
         <v>341</v>
       </c>
@@ -10307,7 +10308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:6" ht="16" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" ht="15">
       <c r="A343" s="1">
         <v>342</v>
       </c>
@@ -10327,7 +10328,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6">
       <c r="A344" s="1">
         <v>343</v>
       </c>
@@ -10344,7 +10345,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6">
       <c r="A345" s="1">
         <v>344</v>
       </c>
@@ -10361,7 +10362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6">
       <c r="A346" s="1">
         <v>345</v>
       </c>
@@ -10381,7 +10382,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6">
       <c r="A347" s="1">
         <v>346</v>
       </c>
@@ -10398,7 +10399,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6">
       <c r="A348" s="1">
         <v>347</v>
       </c>
@@ -10418,7 +10419,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6">
       <c r="A349" s="1">
         <v>348</v>
       </c>
@@ -10435,7 +10436,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6">
       <c r="A350" s="1">
         <v>349</v>
       </c>
@@ -10455,7 +10456,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="351" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" ht="15">
       <c r="A351" s="1">
         <v>350</v>
       </c>
@@ -10472,7 +10473,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="352" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" ht="15">
       <c r="A352" s="1">
         <v>351</v>
       </c>
@@ -10489,7 +10490,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="353" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" ht="15">
       <c r="A353" s="1">
         <v>352</v>
       </c>
@@ -10506,7 +10507,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="354" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" ht="15">
       <c r="A354" s="1">
         <v>353</v>
       </c>
@@ -10523,7 +10524,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6">
       <c r="A355" s="1">
         <v>354</v>
       </c>

</xml_diff>

<commit_message>
update solution for Q.five
</commit_message>
<xml_diff>
--- a/附件四：354个操作变量信息.xlsx
+++ b/附件四：354个操作变量信息.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryuchen/Desktop/2020年B题/数模题/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D131165-4EB1-AD48-BE75-6C445F58223E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8184CF4B-7B93-2745-9384-83D5CFF7180A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1612,9 +1612,6 @@
   </si>
   <si>
     <t>K-101A排气压力</t>
-  </si>
-  <si>
-    <t>S-ZORB.PT_7103.DACA</t>
   </si>
   <si>
     <t>K-101A进气压力</t>
@@ -3529,12 +3526,16 @@
     <t>KPa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>S-ZORB.PT_7103.DACA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3617,6 +3618,15 @@
       <family val="1"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3641,7 +3651,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3665,6 +3675,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3947,13 +3960,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F355"/>
+  <dimension ref="A1:G355"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B332" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H341" sqref="H341"/>
+      <selection pane="bottomRight" activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3968,22 +3981,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>692</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3997,7 +4010,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="F2" s="2">
         <v>0.01</v>
@@ -4014,10 +4027,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -4034,10 +4047,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F4" s="2">
         <v>0.1</v>
@@ -4054,10 +4067,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F5" s="2">
         <v>50</v>
@@ -4074,10 +4087,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -4094,10 +4107,10 @@
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -4114,10 +4127,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F8" s="2">
         <v>0.1</v>
@@ -4134,10 +4147,10 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
@@ -4154,10 +4167,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F10" s="2">
         <v>100</v>
@@ -4174,10 +4187,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F11" s="2">
         <v>2</v>
@@ -4194,10 +4207,10 @@
         <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
@@ -4214,10 +4227,10 @@
         <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F13" s="2">
         <v>0.1</v>
@@ -4234,10 +4247,10 @@
         <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F14" s="2">
         <v>50</v>
@@ -4254,10 +4267,10 @@
         <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F15" s="2">
         <v>0.1</v>
@@ -4274,16 +4287,16 @@
         <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F16" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4294,16 +4307,17 @@
         <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4314,16 +4328,16 @@
         <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4334,16 +4348,16 @@
         <v>34</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="F19" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4354,16 +4368,16 @@
         <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4374,16 +4388,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4394,16 +4408,16 @@
         <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F22" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4414,16 +4428,16 @@
         <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4434,16 +4448,16 @@
         <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F24" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4454,16 +4468,16 @@
         <v>46</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F25" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4474,16 +4488,16 @@
         <v>48</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F26" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4494,16 +4508,16 @@
         <v>50</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F27" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4514,16 +4528,16 @@
         <v>52</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F28" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4534,16 +4548,16 @@
         <v>54</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F29" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -4554,16 +4568,16 @@
         <v>56</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F30" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -4574,16 +4588,16 @@
         <v>58</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F31" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4594,10 +4608,10 @@
         <v>60</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F32" s="2">
         <v>50</v>
@@ -4614,10 +4628,10 @@
         <v>62</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F33" s="2">
         <v>50</v>
@@ -4634,10 +4648,10 @@
         <v>64</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F34" s="2">
         <v>0.05</v>
@@ -4654,10 +4668,10 @@
         <v>66</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
@@ -4674,10 +4688,10 @@
         <v>68</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F36" s="2">
         <v>50</v>
@@ -4694,10 +4708,10 @@
         <v>70</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F37" s="2">
         <v>50</v>
@@ -4714,10 +4728,10 @@
         <v>72</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F38" s="2">
         <v>50</v>
@@ -4734,10 +4748,10 @@
         <v>74</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F39" s="2">
         <v>50</v>
@@ -4754,10 +4768,10 @@
         <v>76</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F40" s="2">
         <v>50</v>
@@ -4774,10 +4788,10 @@
         <v>78</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F41" s="2">
         <v>0.05</v>
@@ -4794,10 +4808,10 @@
         <v>80</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F42" s="2">
         <v>50</v>
@@ -4814,10 +4828,10 @@
         <v>82</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F43" s="2">
         <v>0.05</v>
@@ -4834,10 +4848,10 @@
         <v>84</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F44" s="2">
         <v>-5</v>
@@ -4854,10 +4868,10 @@
         <v>86</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F45" s="2">
         <v>5</v>
@@ -4874,10 +4888,10 @@
         <v>88</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F46" s="2">
         <v>5</v>
@@ -4894,10 +4908,10 @@
         <v>90</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F47" s="2">
         <v>5</v>
@@ -4914,10 +4928,10 @@
         <v>92</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F48" s="2">
         <v>5</v>
@@ -4934,10 +4948,10 @@
         <v>94</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F49" s="2">
         <v>5</v>
@@ -4954,10 +4968,10 @@
         <v>96</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>976</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>977</v>
       </c>
       <c r="F50" s="2">
         <v>10</v>
@@ -4974,10 +4988,10 @@
         <v>98</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F51" s="2">
         <v>1</v>
@@ -4994,10 +5008,10 @@
         <v>100</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F52" s="2">
         <v>10</v>
@@ -5014,10 +5028,10 @@
         <v>102</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F53" s="2">
         <v>0.5</v>
@@ -5034,10 +5048,10 @@
         <v>104</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F54" s="2">
         <v>100</v>
@@ -5054,10 +5068,10 @@
         <v>106</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F55" s="2">
         <v>10</v>
@@ -5074,10 +5088,10 @@
         <v>108</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F56" s="2">
         <v>1</v>
@@ -5094,10 +5108,10 @@
         <v>110</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F57" s="2">
         <v>0.05</v>
@@ -5114,10 +5128,10 @@
         <v>112</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F58" s="2">
         <v>1</v>
@@ -5131,13 +5145,13 @@
         <v>113</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F59" s="2">
         <v>1</v>
@@ -5154,7 +5168,7 @@
         <v>115</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F60" s="2">
         <v>-0.05</v>
@@ -5171,10 +5185,10 @@
         <v>117</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F61" s="2">
         <v>0.05</v>
@@ -5191,10 +5205,10 @@
         <v>119</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F62" s="2">
         <v>1</v>
@@ -5208,13 +5222,13 @@
         <v>120</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F63" s="2">
         <v>1</v>
@@ -5231,7 +5245,7 @@
         <v>122</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F64" s="2">
         <v>-0.1</v>
@@ -5248,10 +5262,10 @@
         <v>124</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F65" s="2">
         <v>0.05</v>
@@ -5268,10 +5282,10 @@
         <v>126</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F66" s="2">
         <v>0.1</v>
@@ -5288,10 +5302,10 @@
         <v>128</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F67" s="2">
         <v>0.1</v>
@@ -5308,10 +5322,10 @@
         <v>130</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F68" s="2">
         <v>0.1</v>
@@ -5328,10 +5342,10 @@
         <v>132</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F69" s="2">
         <v>5</v>
@@ -5348,10 +5362,10 @@
         <v>134</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F70" s="2">
         <v>5</v>
@@ -5368,10 +5382,10 @@
         <v>136</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F71" s="2">
         <v>1</v>
@@ -5388,10 +5402,10 @@
         <v>138</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F72" s="2">
         <v>1</v>
@@ -5408,10 +5422,10 @@
         <v>140</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F73" s="2">
         <v>5</v>
@@ -5428,10 +5442,10 @@
         <v>142</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F74" s="2">
         <v>1</v>
@@ -5448,10 +5462,10 @@
         <v>144</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F75" s="2">
         <v>30</v>
@@ -5468,10 +5482,10 @@
         <v>146</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F76" s="2">
         <v>0.1</v>
@@ -5488,10 +5502,10 @@
         <v>148</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F77" s="2">
         <v>1</v>
@@ -5508,10 +5522,10 @@
         <v>150</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F78" s="2">
         <v>50</v>
@@ -5528,10 +5542,10 @@
         <v>152</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F79" s="2">
         <v>10</v>
@@ -5548,10 +5562,10 @@
         <v>154</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F80" s="2">
         <v>10</v>
@@ -5568,10 +5582,10 @@
         <v>156</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F81" s="2">
         <v>0.05</v>
@@ -5588,10 +5602,10 @@
         <v>158</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F82" s="2">
         <v>5</v>
@@ -5608,10 +5622,10 @@
         <v>160</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F83" s="2">
         <v>1</v>
@@ -5628,10 +5642,10 @@
         <v>162</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F84" s="2">
         <v>1</v>
@@ -5648,10 +5662,10 @@
         <v>164</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F85" s="2">
         <v>0.2</v>
@@ -5668,10 +5682,10 @@
         <v>166</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F86" s="2">
         <v>5</v>
@@ -5688,10 +5702,10 @@
         <v>168</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F87" s="2">
         <v>2</v>
@@ -5705,10 +5719,10 @@
         <v>169</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F88" s="2">
         <v>1000</v>
@@ -5722,7 +5736,7 @@
         <v>170</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F89" s="2">
         <v>0.2</v>
@@ -5736,7 +5750,7 @@
         <v>171</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F90" s="2">
         <v>10</v>
@@ -5750,7 +5764,7 @@
         <v>172</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="F91" s="2">
         <v>10000</v>
@@ -5764,7 +5778,7 @@
         <v>173</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F92" s="2">
         <v>10000</v>
@@ -5778,7 +5792,7 @@
         <v>174</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="F93" s="2">
         <v>500</v>
@@ -5792,7 +5806,7 @@
         <v>175</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F94" s="2">
         <v>10000</v>
@@ -5806,7 +5820,7 @@
         <v>176</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="F95" s="2">
         <v>10000</v>
@@ -5820,7 +5834,7 @@
         <v>177</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="F96" s="2">
         <v>10000</v>
@@ -5837,10 +5851,10 @@
         <v>48</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F97" s="2">
         <v>10000</v>
@@ -5854,7 +5868,7 @@
         <v>179</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="F98" s="2">
         <v>10000</v>
@@ -5868,7 +5882,7 @@
         <v>180</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="F99" s="2">
         <v>1000</v>
@@ -5882,7 +5896,7 @@
         <v>181</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F100" s="2">
         <v>10000</v>
@@ -5896,7 +5910,7 @@
         <v>182</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F101" s="2">
         <v>10000</v>
@@ -5910,7 +5924,7 @@
         <v>183</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="F102" s="2">
         <v>2000</v>
@@ -5924,7 +5938,7 @@
         <v>184</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F103" s="2">
         <v>2000</v>
@@ -5938,7 +5952,7 @@
         <v>185</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F104" s="2">
         <v>10000</v>
@@ -5952,7 +5966,7 @@
         <v>186</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F105" s="2">
         <v>10000</v>
@@ -5966,7 +5980,7 @@
         <v>187</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F106" s="2">
         <v>10000</v>
@@ -5980,7 +5994,7 @@
         <v>188</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="15">
@@ -5991,13 +6005,13 @@
         <v>189</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F108" s="2">
         <v>10</v>
@@ -6014,10 +6028,10 @@
         <v>191</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F109" s="2">
         <v>10000</v>
@@ -6031,7 +6045,7 @@
         <v>192</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="F110" s="2">
         <v>10</v>
@@ -6045,7 +6059,7 @@
         <v>193</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="F111" s="2">
         <v>10</v>
@@ -6059,7 +6073,7 @@
         <v>194</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F112" s="2">
         <v>10000</v>
@@ -6073,7 +6087,7 @@
         <v>195</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F113" s="2">
         <v>10000</v>
@@ -6090,10 +6104,10 @@
         <v>197</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F114" s="2">
         <v>10000</v>
@@ -6110,7 +6124,7 @@
         <v>199</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F115" s="2">
         <v>10000</v>
@@ -6127,10 +6141,10 @@
         <v>201</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F116" s="2">
         <v>10000</v>
@@ -6147,10 +6161,10 @@
         <v>203</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F117" s="2">
         <v>1</v>
@@ -6167,10 +6181,10 @@
         <v>205</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F118" s="2">
         <v>0.1</v>
@@ -6187,10 +6201,10 @@
         <v>207</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F119" s="2">
         <v>0.1</v>
@@ -6207,10 +6221,10 @@
         <v>209</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F120" s="2">
         <v>1</v>
@@ -6227,10 +6241,10 @@
         <v>211</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F121" s="2">
         <v>1</v>
@@ -6247,10 +6261,10 @@
         <v>213</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F122" s="2">
         <v>1</v>
@@ -6267,10 +6281,10 @@
         <v>215</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F123" s="2">
         <v>1</v>
@@ -6287,10 +6301,10 @@
         <v>217</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F124" s="2">
         <v>5</v>
@@ -6307,10 +6321,10 @@
         <v>219</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F125" s="2">
         <v>1</v>
@@ -6327,10 +6341,10 @@
         <v>221</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F126" s="2">
         <v>1</v>
@@ -6347,10 +6361,10 @@
         <v>223</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F127" s="2">
         <v>30</v>
@@ -6367,7 +6381,7 @@
         <v>225</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F128" s="2">
         <v>0.1</v>
@@ -6384,7 +6398,7 @@
         <v>227</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="F129" s="2">
         <v>0.3</v>
@@ -6401,10 +6415,10 @@
         <v>229</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="F130" s="2">
         <v>5</v>
@@ -6421,7 +6435,7 @@
         <v>231</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="F131" s="2">
         <v>5</v>
@@ -6438,10 +6452,10 @@
         <v>233</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="F132" s="2">
         <v>0.2</v>
@@ -6458,10 +6472,10 @@
         <v>235</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="F133" s="2">
         <v>0.5</v>
@@ -6478,10 +6492,10 @@
         <v>237</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F134" s="2">
         <v>0.05</v>
@@ -6498,10 +6512,10 @@
         <v>239</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F135" s="2">
         <v>1</v>
@@ -6518,10 +6532,10 @@
         <v>241</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F136" s="2">
         <v>50</v>
@@ -6538,10 +6552,10 @@
         <v>243</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="F137" s="2">
         <v>5</v>
@@ -6558,10 +6572,10 @@
         <v>245</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F138" s="2">
         <v>0.1</v>
@@ -6578,7 +6592,7 @@
         <v>247</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F139" s="2">
         <v>200</v>
@@ -6595,10 +6609,10 @@
         <v>249</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -6612,10 +6626,10 @@
         <v>251</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F141" s="2">
         <v>1</v>
@@ -6632,10 +6646,10 @@
         <v>253</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F142" s="2">
         <v>1</v>
@@ -6652,10 +6666,10 @@
         <v>255</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="F143" s="2">
         <v>2</v>
@@ -6672,10 +6686,10 @@
         <v>257</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -6689,7 +6703,7 @@
         <v>259</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F145" s="2">
         <v>10</v>
@@ -6706,7 +6720,7 @@
         <v>261</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F146" s="2">
         <v>5</v>
@@ -6723,10 +6737,10 @@
         <v>263</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F147" s="2">
         <v>100</v>
@@ -6743,7 +6757,7 @@
         <v>265</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F148" s="2">
         <v>5</v>
@@ -6760,7 +6774,7 @@
         <v>267</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F149" s="2">
         <v>5</v>
@@ -6777,7 +6791,7 @@
         <v>269</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F150" s="2">
         <v>0.05</v>
@@ -6794,7 +6808,7 @@
         <v>271</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F151" s="2">
         <v>5</v>
@@ -6811,7 +6825,7 @@
         <v>273</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F152" s="2">
         <v>5</v>
@@ -6828,10 +6842,10 @@
         <v>275</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F153" s="2">
         <v>1</v>
@@ -6848,7 +6862,7 @@
         <v>277</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F154" s="2">
         <v>5</v>
@@ -6865,7 +6879,7 @@
         <v>279</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F155" s="2">
         <v>5</v>
@@ -6882,10 +6896,10 @@
         <v>281</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F156" s="2">
         <v>1</v>
@@ -6902,7 +6916,7 @@
         <v>283</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="F157" s="2">
         <v>0.05</v>
@@ -6919,7 +6933,7 @@
         <v>285</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F158" s="2">
         <v>0.05</v>
@@ -6936,7 +6950,7 @@
         <v>287</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F159" s="2">
         <v>1000</v>
@@ -6953,7 +6967,7 @@
         <v>289</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="F160" s="2">
         <v>10</v>
@@ -6970,7 +6984,7 @@
         <v>291</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F161" s="2">
         <v>1</v>
@@ -6987,10 +7001,10 @@
         <v>293</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F162" s="2">
         <v>1</v>
@@ -7007,7 +7021,7 @@
         <v>295</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F163" s="2">
         <v>5</v>
@@ -7024,10 +7038,10 @@
         <v>297</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F164" s="2">
         <v>5</v>
@@ -7044,10 +7058,10 @@
         <v>299</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F165" s="2">
         <v>20</v>
@@ -7064,10 +7078,10 @@
         <v>301</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F166" s="2">
         <v>1</v>
@@ -7084,10 +7098,10 @@
         <v>303</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F167" s="2">
         <v>1</v>
@@ -7104,7 +7118,7 @@
         <v>305</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F168" s="2">
         <v>1</v>
@@ -7121,10 +7135,10 @@
         <v>307</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F169" s="2">
         <v>1</v>
@@ -7141,10 +7155,10 @@
         <v>309</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F170" s="2">
         <v>1</v>
@@ -7161,7 +7175,7 @@
         <v>311</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="F171" s="2">
         <v>10000</v>
@@ -7178,10 +7192,10 @@
         <v>313</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F172" s="2">
         <v>1</v>
@@ -7198,10 +7212,10 @@
         <v>315</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F173" s="2">
         <v>1</v>
@@ -7218,10 +7232,10 @@
         <v>317</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F174" s="2">
         <v>1</v>
@@ -7238,10 +7252,10 @@
         <v>319</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F175" s="2">
         <v>1</v>
@@ -7255,7 +7269,7 @@
         <v>320</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="F176" s="2">
         <v>100</v>
@@ -7272,7 +7286,7 @@
         <v>322</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F177" s="2">
         <v>50</v>
@@ -7289,7 +7303,7 @@
         <v>322</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="F178" s="2">
         <v>1</v>
@@ -7306,7 +7320,7 @@
         <v>325</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F179" s="2">
         <v>50</v>
@@ -7323,10 +7337,10 @@
         <v>327</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F180" s="2">
         <v>10</v>
@@ -7343,10 +7357,10 @@
         <v>329</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F181" s="2">
         <v>10</v>
@@ -7363,10 +7377,10 @@
         <v>329</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F182" s="2">
         <v>1</v>
@@ -7383,7 +7397,7 @@
         <v>332</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F183" s="2">
         <v>5</v>
@@ -7400,7 +7414,7 @@
         <v>334</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F184" s="2">
         <v>0.05</v>
@@ -7417,7 +7431,7 @@
         <v>336</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F185" s="2">
         <v>5</v>
@@ -7434,7 +7448,7 @@
         <v>338</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F186" s="2">
         <v>0.1</v>
@@ -7451,7 +7465,7 @@
         <v>340</v>
       </c>
       <c r="D187" s="4" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F187" s="2">
         <v>10</v>
@@ -7468,10 +7482,10 @@
         <v>342</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F188" s="2">
         <v>0.1</v>
@@ -7488,7 +7502,7 @@
         <v>344</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F189" s="2">
         <v>1</v>
@@ -7505,7 +7519,7 @@
         <v>346</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F190" s="2">
         <v>1</v>
@@ -7522,10 +7536,10 @@
         <v>348</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F191" s="2">
         <v>1</v>
@@ -7542,10 +7556,10 @@
         <v>350</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F192" s="2">
         <v>1</v>
@@ -7562,10 +7576,10 @@
         <v>352</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F193" s="2">
         <v>0.1</v>
@@ -7582,7 +7596,7 @@
         <v>354</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F194" s="2">
         <v>0.1</v>
@@ -7599,10 +7613,10 @@
         <v>356</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F195" s="2">
         <v>0.05</v>
@@ -7619,7 +7633,7 @@
         <v>358</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F196" s="2">
         <v>1000</v>
@@ -7636,10 +7650,10 @@
         <v>360</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F197" s="2">
         <v>1</v>
@@ -7656,10 +7670,10 @@
         <v>362</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F198" s="2">
         <v>50</v>
@@ -7676,7 +7690,7 @@
         <v>364</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="F199" s="2">
         <v>0.1</v>
@@ -7693,7 +7707,7 @@
         <v>366</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F200" s="2">
         <v>0.1</v>
@@ -7710,10 +7724,10 @@
         <v>368</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F201" s="2">
         <v>0.1</v>
@@ -7730,10 +7744,10 @@
         <v>370</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F202" s="2">
         <v>20</v>
@@ -7750,10 +7764,10 @@
         <v>372</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F203" s="2">
         <v>100</v>
@@ -7770,10 +7784,10 @@
         <v>374</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E204" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F204" s="2">
         <v>5</v>
@@ -7790,7 +7804,7 @@
         <v>376</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F205" s="2">
         <v>0.05</v>
@@ -7807,7 +7821,7 @@
         <v>378</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F206" s="2">
         <v>0.1</v>
@@ -7824,7 +7838,7 @@
         <v>380</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F207" s="2">
         <v>0.2</v>
@@ -7841,10 +7855,10 @@
         <v>382</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F208" s="2">
         <v>5</v>
@@ -7861,10 +7875,10 @@
         <v>384</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F209" s="2">
         <v>0.5</v>
@@ -7881,7 +7895,7 @@
         <v>386</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F210" s="2">
         <v>5</v>
@@ -7898,7 +7912,7 @@
         <v>388</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F211" s="2">
         <v>0.5</v>
@@ -7915,7 +7929,7 @@
         <v>390</v>
       </c>
       <c r="D212" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F212" s="2">
         <v>0.1</v>
@@ -7932,10 +7946,10 @@
         <v>392</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E213" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F213" s="2">
         <v>1</v>
@@ -7952,7 +7966,7 @@
         <v>394</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F214" s="2">
         <v>0.1</v>
@@ -7969,7 +7983,7 @@
         <v>396</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F215" s="2">
         <v>0.1</v>
@@ -7986,7 +8000,7 @@
         <v>398</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F216" s="2">
         <v>0.1</v>
@@ -8003,7 +8017,7 @@
         <v>400</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F217" s="2">
         <v>50</v>
@@ -8020,7 +8034,7 @@
         <v>402</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F218" s="2">
         <v>5</v>
@@ -8037,7 +8051,7 @@
         <v>404</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F219" s="2">
         <v>1</v>
@@ -8054,7 +8068,7 @@
         <v>406</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="F220" s="2">
         <v>0.1</v>
@@ -8071,7 +8085,7 @@
         <v>408</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F221" s="2">
         <v>0.1</v>
@@ -8088,7 +8102,7 @@
         <v>410</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="F222" s="2">
         <v>0.1</v>
@@ -8105,7 +8119,7 @@
         <v>412</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F223" s="2">
         <v>5</v>
@@ -8122,7 +8136,7 @@
         <v>414</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F224" s="2">
         <v>5</v>
@@ -8139,7 +8153,7 @@
         <v>416</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F225" s="2">
         <v>0.05</v>
@@ -8156,7 +8170,7 @@
         <v>418</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F226" s="2">
         <v>10</v>
@@ -8173,7 +8187,7 @@
         <v>420</v>
       </c>
       <c r="D227" s="4" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F227" s="2">
         <v>0.5</v>
@@ -8190,7 +8204,7 @@
         <v>422</v>
       </c>
       <c r="D228" s="4" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F228" s="2">
         <v>0.1</v>
@@ -8207,7 +8221,7 @@
         <v>424</v>
       </c>
       <c r="D229" s="4" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F229" s="2">
         <v>1</v>
@@ -8224,7 +8238,7 @@
         <v>426</v>
       </c>
       <c r="D230" s="4" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F230" s="2">
         <v>5</v>
@@ -8241,10 +8255,10 @@
         <v>428</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F231" s="2">
         <v>5</v>
@@ -8261,10 +8275,10 @@
         <v>430</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E232" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F232" s="2">
         <v>5</v>
@@ -8281,10 +8295,10 @@
         <v>432</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F233" s="2">
         <v>1</v>
@@ -8301,7 +8315,7 @@
         <v>434</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F234" s="2">
         <v>10</v>
@@ -8318,7 +8332,7 @@
         <v>436</v>
       </c>
       <c r="D235" s="4" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F235" s="2">
         <v>1</v>
@@ -8335,10 +8349,10 @@
         <v>438</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E236" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F236" s="2">
         <v>1</v>
@@ -8355,7 +8369,7 @@
         <v>440</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F237" s="2">
         <v>2</v>
@@ -8372,10 +8386,10 @@
         <v>442</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E238" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F238" s="2">
         <v>1</v>
@@ -8392,10 +8406,10 @@
         <v>442</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E239" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F239" s="2">
         <v>1</v>
@@ -8412,10 +8426,10 @@
         <v>445</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E240" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F240" s="2">
         <v>1</v>
@@ -8432,10 +8446,10 @@
         <v>445</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F241" s="2">
         <v>1</v>
@@ -8452,7 +8466,7 @@
         <v>448</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F242" s="2">
         <v>0.1</v>
@@ -8469,7 +8483,7 @@
         <v>450</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F243" s="2">
         <v>5</v>
@@ -8486,7 +8500,7 @@
         <v>452</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F244" s="2">
         <v>10</v>
@@ -8503,7 +8517,7 @@
         <v>454</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F245" s="2">
         <v>0.1</v>
@@ -8520,10 +8534,10 @@
         <v>456</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F246" s="2">
         <v>0.5</v>
@@ -8540,7 +8554,7 @@
         <v>458</v>
       </c>
       <c r="D247" s="4" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F247" s="2">
         <v>1</v>
@@ -8557,7 +8571,7 @@
         <v>460</v>
       </c>
       <c r="D248" s="4" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F248" s="2">
         <v>1</v>
@@ -8574,7 +8588,7 @@
         <v>462</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F249" s="2">
         <v>1</v>
@@ -8591,7 +8605,7 @@
         <v>464</v>
       </c>
       <c r="D250" s="4" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F250" s="2">
         <v>0.1</v>
@@ -8608,7 +8622,7 @@
         <v>466</v>
       </c>
       <c r="D251" s="4" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="F251" s="2">
         <v>1</v>
@@ -8625,7 +8639,7 @@
         <v>468</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F252" s="2">
         <v>1</v>
@@ -8642,7 +8656,7 @@
         <v>470</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F253" s="2">
         <v>1</v>
@@ -8659,7 +8673,7 @@
         <v>472</v>
       </c>
       <c r="D254" s="4" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F254" s="2">
         <v>2</v>
@@ -8676,7 +8690,7 @@
         <v>474</v>
       </c>
       <c r="D255" s="4" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F255" s="2">
         <v>5</v>
@@ -8693,7 +8707,7 @@
         <v>476</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="F256" s="2">
         <v>1</v>
@@ -8710,7 +8724,7 @@
         <v>478</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F257" s="2">
         <v>0.1</v>
@@ -8727,7 +8741,7 @@
         <v>480</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F258" s="2">
         <v>100</v>
@@ -8744,7 +8758,7 @@
         <v>482</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F259" s="2">
         <v>0.1</v>
@@ -8761,10 +8775,10 @@
         <v>484</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E260" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F260" s="2">
         <v>1</v>
@@ -8781,7 +8795,7 @@
         <v>486</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="F261" s="2">
         <v>0.2</v>
@@ -8798,10 +8812,10 @@
         <v>488</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E262" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F262" s="2">
         <v>1</v>
@@ -8818,7 +8832,7 @@
         <v>490</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="F263" s="2">
         <v>1000</v>
@@ -8835,10 +8849,10 @@
         <v>492</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E264" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F264" s="2">
         <v>1</v>
@@ -8855,7 +8869,7 @@
         <v>494</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="F265" s="2">
         <v>1000</v>
@@ -8872,10 +8886,10 @@
         <v>496</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E266" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F266" s="2">
         <v>1</v>
@@ -8892,7 +8906,7 @@
         <v>498</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F267" s="2">
         <v>0.2</v>
@@ -8909,10 +8923,10 @@
         <v>500</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E268" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F268" s="2">
         <v>1</v>
@@ -8929,7 +8943,7 @@
         <v>502</v>
       </c>
       <c r="D269" s="4" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F269" s="2">
         <v>0.1</v>
@@ -8946,10 +8960,10 @@
         <v>504</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E270" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F270" s="2">
         <v>1</v>
@@ -8966,7 +8980,7 @@
         <v>506</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="F271" s="2">
         <v>1</v>
@@ -8983,10 +8997,10 @@
         <v>508</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E272" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F272" s="2">
         <v>1</v>
@@ -9003,7 +9017,7 @@
         <v>510</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="F273" s="2">
         <v>1</v>
@@ -9020,10 +9034,10 @@
         <v>512</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E274" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F274" s="2">
         <v>1</v>
@@ -9040,10 +9054,10 @@
         <v>514</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E275" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F275" s="2">
         <v>1</v>
@@ -9060,10 +9074,10 @@
         <v>516</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E276" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F276" s="2">
         <v>1</v>
@@ -9080,7 +9094,7 @@
         <v>518</v>
       </c>
       <c r="D277" s="4" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F277" s="2">
         <v>0.05</v>
@@ -9097,7 +9111,7 @@
         <v>520</v>
       </c>
       <c r="D278" s="4" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F278" s="2">
         <v>0.05</v>
@@ -9114,10 +9128,10 @@
         <v>522</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E279" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F279" s="2">
         <v>1</v>
@@ -9134,10 +9148,10 @@
         <v>524</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E280" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F280" s="2">
         <v>1</v>
@@ -9154,10 +9168,10 @@
         <v>526</v>
       </c>
       <c r="D281" s="4" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E281" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F281" s="2">
         <v>1</v>
@@ -9168,13 +9182,13 @@
         <v>281</v>
       </c>
       <c r="B282" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C282" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C282" s="1" t="s">
-        <v>528</v>
-      </c>
       <c r="D282" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F282" s="2">
         <v>100</v>
@@ -9185,13 +9199,13 @@
         <v>282</v>
       </c>
       <c r="B283" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C283" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="C283" s="1" t="s">
-        <v>530</v>
-      </c>
       <c r="D283" s="4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F283" s="2">
         <v>100</v>
@@ -9202,16 +9216,16 @@
         <v>283</v>
       </c>
       <c r="B284" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C284" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="C284" s="1" t="s">
-        <v>532</v>
-      </c>
       <c r="D284" s="4" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E284" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F284" s="2">
         <v>1</v>
@@ -9222,13 +9236,13 @@
         <v>284</v>
       </c>
       <c r="B285" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C285" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="C285" s="1" t="s">
-        <v>534</v>
-      </c>
       <c r="D285" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F285" s="2">
         <v>2</v>
@@ -9239,13 +9253,13 @@
         <v>285</v>
       </c>
       <c r="B286" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C286" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="C286" s="1" t="s">
-        <v>536</v>
-      </c>
       <c r="D286" s="2" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="F286" s="2">
         <v>0.1</v>
@@ -9256,13 +9270,13 @@
         <v>286</v>
       </c>
       <c r="B287" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C287" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="C287" s="1" t="s">
-        <v>538</v>
-      </c>
       <c r="D287" s="4" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="F287" s="2">
         <v>2</v>
@@ -9273,16 +9287,16 @@
         <v>287</v>
       </c>
       <c r="B288" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C288" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="C288" s="1" t="s">
-        <v>540</v>
-      </c>
       <c r="D288" s="4" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E288" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F288" s="2">
         <v>0.1</v>
@@ -9293,13 +9307,13 @@
         <v>288</v>
       </c>
       <c r="B289" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C289" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="C289" s="1" t="s">
-        <v>542</v>
-      </c>
       <c r="D289" s="4" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="F289" s="2">
         <v>0.1</v>
@@ -9310,13 +9324,13 @@
         <v>289</v>
       </c>
       <c r="B290" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C290" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="C290" s="1" t="s">
-        <v>544</v>
-      </c>
       <c r="D290" s="4" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F290" s="2">
         <v>0.1</v>
@@ -9327,13 +9341,13 @@
         <v>290</v>
       </c>
       <c r="B291" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C291" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="C291" s="1" t="s">
-        <v>546</v>
-      </c>
       <c r="D291" s="4" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F291" s="2">
         <v>1</v>
@@ -9344,16 +9358,16 @@
         <v>291</v>
       </c>
       <c r="B292" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C292" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="C292" s="1" t="s">
-        <v>548</v>
-      </c>
       <c r="D292" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E292" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F292" s="2">
         <v>1</v>
@@ -9364,16 +9378,16 @@
         <v>292</v>
       </c>
       <c r="B293" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C293" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C293" s="1" t="s">
-        <v>550</v>
-      </c>
       <c r="D293" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E293" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F293" s="2">
         <v>1</v>
@@ -9384,16 +9398,16 @@
         <v>293</v>
       </c>
       <c r="B294" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C294" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="C294" s="1" t="s">
-        <v>552</v>
-      </c>
       <c r="D294" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E294" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F294" s="2">
         <v>1</v>
@@ -9404,16 +9418,16 @@
         <v>294</v>
       </c>
       <c r="B295" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C295" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="C295" s="1" t="s">
-        <v>554</v>
-      </c>
       <c r="D295" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E295" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F295" s="2">
         <v>1</v>
@@ -9424,16 +9438,16 @@
         <v>295</v>
       </c>
       <c r="B296" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C296" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="C296" s="1" t="s">
-        <v>556</v>
-      </c>
       <c r="D296" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E296" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F296" s="2">
         <v>10</v>
@@ -9444,16 +9458,16 @@
         <v>296</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E297" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F297" s="2">
         <v>1</v>
@@ -9464,16 +9478,16 @@
         <v>297</v>
       </c>
       <c r="B298" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C298" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="C298" s="1" t="s">
-        <v>559</v>
-      </c>
       <c r="D298" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E298" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F298" s="2">
         <v>1</v>
@@ -9484,13 +9498,13 @@
         <v>298</v>
       </c>
       <c r="B299" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C299" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="C299" s="1" t="s">
-        <v>561</v>
-      </c>
       <c r="D299" s="2" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F299" s="2">
         <v>2</v>
@@ -9501,16 +9515,16 @@
         <v>299</v>
       </c>
       <c r="B300" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C300" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="C300" s="1" t="s">
-        <v>563</v>
-      </c>
       <c r="D300" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E300" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F300" s="2">
         <v>1</v>
@@ -9521,16 +9535,16 @@
         <v>300</v>
       </c>
       <c r="B301" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C301" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="C301" s="1" t="s">
-        <v>565</v>
-      </c>
       <c r="D301" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E301" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F301" s="2">
         <v>1</v>
@@ -9541,16 +9555,16 @@
         <v>301</v>
       </c>
       <c r="B302" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C302" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="C302" s="1" t="s">
-        <v>567</v>
-      </c>
       <c r="D302" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E302" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F302" s="2">
         <v>1</v>
@@ -9561,13 +9575,13 @@
         <v>302</v>
       </c>
       <c r="B303" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C303" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="C303" s="1" t="s">
-        <v>569</v>
-      </c>
       <c r="D303" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F303" s="2">
         <v>2</v>
@@ -9578,16 +9592,16 @@
         <v>303</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E304" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F304" s="2">
         <v>1</v>
@@ -9598,16 +9612,16 @@
         <v>304</v>
       </c>
       <c r="B305" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="C305" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="C305" s="1" t="s">
-        <v>572</v>
-      </c>
       <c r="D305" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E305" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F305" s="2">
         <v>1</v>
@@ -9618,16 +9632,16 @@
         <v>305</v>
       </c>
       <c r="B306" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="C306" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="C306" s="1" t="s">
-        <v>574</v>
-      </c>
       <c r="D306" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E306" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F306" s="2">
         <v>1</v>
@@ -9638,16 +9652,16 @@
         <v>306</v>
       </c>
       <c r="B307" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C307" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="C307" s="1" t="s">
-        <v>576</v>
-      </c>
       <c r="D307" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E307" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F307" s="2">
         <v>1</v>
@@ -9658,16 +9672,16 @@
         <v>307</v>
       </c>
       <c r="B308" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C308" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="C308" s="1" t="s">
-        <v>578</v>
-      </c>
       <c r="D308" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E308" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F308" s="2">
         <v>1</v>
@@ -9678,16 +9692,16 @@
         <v>308</v>
       </c>
       <c r="B309" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C309" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="C309" s="1" t="s">
-        <v>580</v>
-      </c>
       <c r="D309" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E309" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F309" s="2">
         <v>1</v>
@@ -9698,16 +9712,16 @@
         <v>309</v>
       </c>
       <c r="B310" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="C310" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="C310" s="1" t="s">
-        <v>582</v>
-      </c>
       <c r="D310" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E310" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F310" s="2">
         <v>1</v>
@@ -9718,16 +9732,16 @@
         <v>310</v>
       </c>
       <c r="B311" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C311" s="1" t="s">
         <v>583</v>
       </c>
-      <c r="C311" s="1" t="s">
-        <v>584</v>
-      </c>
       <c r="D311" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E311" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F311" s="2">
         <v>1</v>
@@ -9738,16 +9752,16 @@
         <v>311</v>
       </c>
       <c r="B312" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C312" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="C312" s="1" t="s">
-        <v>586</v>
-      </c>
       <c r="D312" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E312" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F312" s="2">
         <v>1</v>
@@ -9758,16 +9772,16 @@
         <v>312</v>
       </c>
       <c r="B313" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C313" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="C313" s="1" t="s">
-        <v>588</v>
-      </c>
       <c r="D313" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E313" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F313" s="2">
         <v>0.1</v>
@@ -9778,13 +9792,13 @@
         <v>313</v>
       </c>
       <c r="B314" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C314" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="C314" s="1" t="s">
-        <v>590</v>
-      </c>
       <c r="D314" s="2" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F314" s="2">
         <v>1</v>
@@ -9795,13 +9809,13 @@
         <v>314</v>
       </c>
       <c r="B315" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C315" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="C315" s="1" t="s">
-        <v>592</v>
-      </c>
       <c r="D315" s="2" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F315" s="2">
         <v>1</v>
@@ -9812,13 +9826,13 @@
         <v>315</v>
       </c>
       <c r="B316" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C316" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="C316" s="1" t="s">
-        <v>594</v>
-      </c>
       <c r="D316" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F316" s="2">
         <v>0.1</v>
@@ -9829,13 +9843,13 @@
         <v>316</v>
       </c>
       <c r="B317" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C317" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="C317" s="1" t="s">
-        <v>596</v>
-      </c>
       <c r="D317" s="2" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F317" s="2">
         <v>0.1</v>
@@ -9846,13 +9860,13 @@
         <v>317</v>
       </c>
       <c r="B318" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C318" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="C318" s="1" t="s">
-        <v>598</v>
-      </c>
       <c r="D318" s="2" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F318" s="2">
         <v>0.1</v>
@@ -9863,13 +9877,13 @@
         <v>318</v>
       </c>
       <c r="B319" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C319" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="C319" s="1" t="s">
-        <v>600</v>
-      </c>
       <c r="D319" s="2" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F319" s="2">
         <v>0.1</v>
@@ -9880,13 +9894,13 @@
         <v>319</v>
       </c>
       <c r="B320" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C320" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="C320" s="1" t="s">
-        <v>602</v>
-      </c>
       <c r="D320" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F320" s="2">
         <v>0.1</v>
@@ -9897,13 +9911,13 @@
         <v>320</v>
       </c>
       <c r="B321" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C321" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="C321" s="1" t="s">
-        <v>604</v>
-      </c>
       <c r="D321" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F321" s="2">
         <v>0.1</v>
@@ -9914,13 +9928,13 @@
         <v>321</v>
       </c>
       <c r="B322" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C322" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="C322" s="1" t="s">
-        <v>606</v>
-      </c>
       <c r="D322" s="2" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F322" s="2">
         <v>0.1</v>
@@ -9931,13 +9945,13 @@
         <v>322</v>
       </c>
       <c r="B323" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C323" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="C323" s="1" t="s">
-        <v>608</v>
-      </c>
       <c r="D323" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F323" s="2">
         <v>0.1</v>
@@ -9948,13 +9962,13 @@
         <v>323</v>
       </c>
       <c r="B324" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="C324" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="C324" s="1" t="s">
-        <v>610</v>
-      </c>
       <c r="D324" s="2" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="F324" s="2">
         <v>0.1</v>
@@ -9965,13 +9979,13 @@
         <v>324</v>
       </c>
       <c r="B325" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="C325" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="C325" s="1" t="s">
-        <v>612</v>
-      </c>
       <c r="D325" s="2" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F325" s="2">
         <v>0.1</v>
@@ -9982,13 +9996,13 @@
         <v>325</v>
       </c>
       <c r="B326" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="C326" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="C326" s="1" t="s">
-        <v>614</v>
-      </c>
       <c r="D326" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F326" s="2">
         <v>1</v>
@@ -9999,16 +10013,16 @@
         <v>326</v>
       </c>
       <c r="B327" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="C327" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="C327" s="1" t="s">
-        <v>616</v>
-      </c>
       <c r="D327" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E327" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F327" s="2">
         <v>1</v>
@@ -10019,16 +10033,16 @@
         <v>327</v>
       </c>
       <c r="B328" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C328" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="C328" s="1" t="s">
-        <v>618</v>
-      </c>
       <c r="D328" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E328" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F328" s="2">
         <v>0.1</v>
@@ -10039,13 +10053,13 @@
         <v>328</v>
       </c>
       <c r="B329" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="C329" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="C329" s="1" t="s">
-        <v>620</v>
-      </c>
       <c r="D329" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F329" s="2">
         <v>2</v>
@@ -10056,16 +10070,16 @@
         <v>329</v>
       </c>
       <c r="B330" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="C330" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="C330" s="1" t="s">
-        <v>622</v>
-      </c>
       <c r="D330" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E330" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F330" s="2">
         <v>2</v>
@@ -10076,16 +10090,16 @@
         <v>330</v>
       </c>
       <c r="B331" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="C331" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="C331" s="1" t="s">
-        <v>624</v>
-      </c>
       <c r="D331" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E331" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F331" s="2">
         <v>2</v>
@@ -10096,16 +10110,16 @@
         <v>331</v>
       </c>
       <c r="B332" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="C332" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="C332" s="1" t="s">
-        <v>626</v>
-      </c>
       <c r="D332" s="2" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E332" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="F332" s="2">
         <v>2</v>
@@ -10116,13 +10130,13 @@
         <v>332</v>
       </c>
       <c r="B333" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="C333" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="C333" s="1" t="s">
-        <v>628</v>
-      </c>
       <c r="D333" s="2" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F333" s="2">
         <v>10</v>
@@ -10133,16 +10147,16 @@
         <v>333</v>
       </c>
       <c r="B334" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="C334" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="C334" s="1" t="s">
-        <v>630</v>
-      </c>
       <c r="D334" s="2" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="E334" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="F334" s="2">
         <v>5</v>
@@ -10153,16 +10167,16 @@
         <v>334</v>
       </c>
       <c r="B335" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="C335" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="C335" s="1" t="s">
-        <v>632</v>
-      </c>
       <c r="D335" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="E335" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F335" s="2">
         <v>2</v>
@@ -10173,16 +10187,16 @@
         <v>335</v>
       </c>
       <c r="B336" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="C336" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="C336" s="1" t="s">
-        <v>634</v>
-      </c>
       <c r="D336" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E336" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F336" s="2">
         <v>1</v>
@@ -10193,16 +10207,16 @@
         <v>336</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E337" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F337" s="2">
         <v>1</v>
@@ -10213,16 +10227,16 @@
         <v>337</v>
       </c>
       <c r="B338" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="C338" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="C338" s="1" t="s">
-        <v>637</v>
-      </c>
       <c r="D338" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E338" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F338" s="2">
         <v>2</v>
@@ -10233,16 +10247,16 @@
         <v>338</v>
       </c>
       <c r="B339" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="C339" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="C339" s="1" t="s">
-        <v>639</v>
-      </c>
       <c r="D339" s="4" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E339" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F339" s="2">
         <v>1</v>
@@ -10253,16 +10267,16 @@
         <v>339</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C340" s="1" t="s">
         <v>203</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E340" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F340" s="2">
         <v>1</v>
@@ -10273,16 +10287,16 @@
         <v>340</v>
       </c>
       <c r="B341" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C341" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="C341" s="1" t="s">
-        <v>642</v>
-      </c>
       <c r="D341" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E341" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F341" s="2">
         <v>0.01</v>
@@ -10293,16 +10307,16 @@
         <v>341</v>
       </c>
       <c r="B342" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C342" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="C342" s="1" t="s">
-        <v>644</v>
-      </c>
       <c r="D342" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E342" s="2" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="F342" s="2">
         <v>1</v>
@@ -10313,16 +10327,16 @@
         <v>342</v>
       </c>
       <c r="B343" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="C343" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="C343" s="1" t="s">
-        <v>646</v>
-      </c>
       <c r="D343" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E343" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="F343" s="2">
         <v>0.5</v>
@@ -10333,13 +10347,13 @@
         <v>343</v>
       </c>
       <c r="B344" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="C344" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="C344" s="1" t="s">
-        <v>648</v>
-      </c>
       <c r="D344" s="4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="F344" s="2">
         <v>100</v>
@@ -10350,13 +10364,13 @@
         <v>344</v>
       </c>
       <c r="B345" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="C345" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="C345" s="1" t="s">
-        <v>650</v>
-      </c>
       <c r="D345" s="2" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="F345" s="2">
         <v>1</v>
@@ -10367,16 +10381,16 @@
         <v>345</v>
       </c>
       <c r="B346" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="C346" s="3" t="s">
         <v>651</v>
       </c>
-      <c r="C346" s="3" t="s">
-        <v>652</v>
-      </c>
       <c r="D346" s="2" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="E346" s="2" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="F346" s="2">
         <v>0.2</v>
@@ -10387,13 +10401,13 @@
         <v>346</v>
       </c>
       <c r="B347" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C347" s="3" t="s">
         <v>653</v>
       </c>
-      <c r="C347" s="3" t="s">
-        <v>654</v>
-      </c>
       <c r="D347" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F347" s="2">
         <v>100</v>
@@ -10404,16 +10418,16 @@
         <v>347</v>
       </c>
       <c r="B348" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="C348" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="C348" s="1" t="s">
-        <v>656</v>
-      </c>
       <c r="D348" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E348" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F348" s="2">
         <v>100</v>
@@ -10424,13 +10438,13 @@
         <v>348</v>
       </c>
       <c r="B349" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="C349" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="C349" s="1" t="s">
-        <v>658</v>
-      </c>
       <c r="D349" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F349" s="2">
         <v>10000</v>
@@ -10441,16 +10455,16 @@
         <v>349</v>
       </c>
       <c r="B350" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="C350" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="C350" s="1" t="s">
-        <v>660</v>
-      </c>
       <c r="D350" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E350" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F350" s="2">
         <v>10000</v>
@@ -10461,13 +10475,13 @@
         <v>350</v>
       </c>
       <c r="B351" s="6" t="s">
+        <v>660</v>
+      </c>
+      <c r="C351" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="C351" s="6" t="s">
-        <v>662</v>
-      </c>
       <c r="D351" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F351" s="2">
         <v>10000</v>
@@ -10478,13 +10492,13 @@
         <v>351</v>
       </c>
       <c r="B352" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C352" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D352" s="2" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="F352" s="2">
         <v>10000</v>
@@ -10495,13 +10509,13 @@
         <v>352</v>
       </c>
       <c r="B353" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="C353" s="6" t="s">
         <v>664</v>
       </c>
-      <c r="C353" s="6" t="s">
-        <v>665</v>
-      </c>
       <c r="D353" s="4" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="F353" s="2">
         <v>1000</v>
@@ -10512,13 +10526,13 @@
         <v>353</v>
       </c>
       <c r="B354" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C354" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D354" s="4" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="F354" s="2">
         <v>10000</v>
@@ -10529,13 +10543,13 @@
         <v>354</v>
       </c>
       <c r="B355" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="C355" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="C355" s="7" t="s">
-        <v>668</v>
-      </c>
       <c r="D355" s="4" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F355" s="2">
         <v>0.5</v>

</xml_diff>